<commit_message>
Day 7 solution and run times
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -39,7 +39,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -86,8 +86,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -517,12 +517,16 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1">
+        <v>7.2996999952010802E-3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4.4668999908026299E-3</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.176659998600371E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -767,16 +771,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>1.6116800004965601E-2</v>
+        <v>2.3416500000166682E-2</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>2.8706999873975257E-3</v>
+        <v>7.3375999782001556E-3</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>1.8987499992363127E-2</v>
+        <v>3.0754099978366839E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 8 solution and runtimes
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -385,7 +385,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -534,12 +536,16 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="1">
+        <v>3.05653999967034E-2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4.9919998855329996E-4</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.1064599985256701E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -771,16 +777,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>2.3416500000166682E-2</v>
+        <v>5.3981899996870086E-2</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>7.3375999782001556E-3</v>
+        <v>7.8367999667534553E-3</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>3.0754099978366839E-2</v>
+        <v>6.181869996362354E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 9 Solution and updated runtimes
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -553,12 +553,16 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="B13" s="1">
+        <v>7.9774999758228608E-3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4.3600000208243701E-4</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.413499977905298E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -777,16 +781,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>5.3981899996870086E-2</v>
+        <v>6.1959399972692945E-2</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>7.8367999667534553E-3</v>
+        <v>8.2727999688358925E-3</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>6.181869996362354E-2</v>
+        <v>7.0232199941528836E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 10 Solution and updated runtimes
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,12 +570,16 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1">
+        <v>1.4606699987780299E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7.2334899974521194E-2</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.6941599962301497E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -781,16 +785,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>6.1959399972692945E-2</v>
+        <v>7.6566099960473241E-2</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>8.2727999688358925E-3</v>
+        <v>8.0607699943357092E-2</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>7.0232199941528836E-2</v>
+        <v>0.15717379990383035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised Day 10 Solution
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -571,15 +571,15 @@
         <v>10</v>
       </c>
       <c r="B14" s="1">
-        <v>1.4606699987780299E-2</v>
+        <v>1.31570000085048E-2</v>
       </c>
       <c r="C14" s="1">
-        <v>7.2334899974521194E-2</v>
+        <v>3.0266999965533601E-3</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>8.6941599962301497E-2</v>
+        <v>1.6183700005058161E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -785,16 +785,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>7.6566099960473241E-2</v>
+        <v>7.5116399981197748E-2</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>8.0607699943357092E-2</v>
+        <v>1.1299499965389252E-2</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>0.15717379990383035</v>
+        <v>8.6415899946586994E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day11 Solution and updated runtimes
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -587,12 +587,16 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="1">
+        <v>0.36863070004619602</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6.4990000100806301E-4</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.36928060004720409</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -785,16 +789,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>7.5116399981197748E-2</v>
+        <v>0.44374710002739376</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>1.1299499965389252E-2</v>
+        <v>1.1949399966397316E-2</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>8.6415899946586994E-2</v>
+        <v>0.45569649999379108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Day 11 solution
Simplified input file processing
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,15 +588,15 @@
         <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>0.36863070004619602</v>
+        <v>0.36832229996798499</v>
       </c>
       <c r="C15" s="1">
-        <v>6.4990000100806301E-4</v>
+        <v>6.1170000117272095E-4</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>0.36928060004720409</v>
+        <v>0.36893399996915771</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -789,16 +789,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>0.44374710002739376</v>
+        <v>0.44343869994918272</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>1.1949399966397316E-2</v>
+        <v>1.1911199966561974E-2</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>0.45569649999379108</v>
+        <v>0.4553498999157447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated AoC Days 1-12 plus runtimes to date
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,15 +588,15 @@
         <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>0.36832229996798499</v>
+        <v>1.1525499983690599E-2</v>
       </c>
       <c r="C15" s="1">
-        <v>6.1170000117272095E-4</v>
+        <f>+E15-B15</f>
+        <v>0.17586580000352039</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>0.36893399996915771</v>
+        <v>0.18739129998721099</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -789,16 +789,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>0.44343869994918272</v>
+        <v>8.6641899964888344E-2</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>1.1911199966561974E-2</v>
+        <v>0.18716529996890965</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>0.4553498999157447</v>
+        <v>0.27380719993379798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 13 Solution + runtimes + updates AoCFramework
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,15 +588,15 @@
         <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>1.1525499983690599E-2</v>
+        <v>5.33150000264868E-2</v>
       </c>
       <c r="C15" s="1">
-        <f>+E15-B15</f>
-        <v>0.17586580000352039</v>
+        <v>4.48399921879172E-4</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1">
-        <v>0.18739129998721099</v>
+        <f t="shared" si="0"/>
+        <v>5.3763399948365972E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -604,12 +604,16 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1">
+        <v>1.1525499983690599E-2</v>
+      </c>
+      <c r="C16" s="1">
+        <f>+E16-B16</f>
+        <v>0.17586580000352039</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.18739129998721099</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -617,12 +621,16 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="B17" s="1">
+        <v>7.4696999508887503E-3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.11200031824409E-4</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.5808999827131594E-3</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -789,16 +797,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>8.6641899964888344E-2</v>
+        <v>0.1474265999422639</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>0.18716529996890965</v>
+        <v>0.18772489992261324</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>0.27380719993379798</v>
+        <v>0.33515149986487713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 14 Solution and runtimes
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -638,12 +638,16 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1">
+        <v>1.4449000009335499E-3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.386416800000006</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.38786170000093956</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -797,16 +801,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>0.1474265999422639</v>
+        <v>0.14887149994319746</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>0.18772489992261324</v>
+        <v>0.57414169992261921</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>0.33515149986487713</v>
+        <v>0.72301319986581669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 16 Solution and runtimes
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -672,12 +672,16 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="B20" s="1">
+        <v>8.1190999771934003E-3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.6652642000117299</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6733832999889233</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -805,16 +809,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>0.15097269993566417</v>
+        <v>0.15909179991285757</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>0.57719619992712867</v>
+        <v>2.2424603999388584</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>0.72816889986279287</v>
+        <v>2.4015521998517162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 17 Solution and runtimes
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,12 +689,16 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1">
+        <v>3.02397709997603</v>
+      </c>
+      <c r="C21" s="1">
+        <v>6.1240000650286599E-4</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.0245894999825329</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -809,16 +813,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>0.15909179991285757</v>
+        <v>3.1830688998888874</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>2.2424603999388584</v>
+        <v>2.2430727999453612</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>2.4015521998517162</v>
+        <v>5.4261416998342487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 19 and 20 Solutions and runtimes
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -740,12 +740,16 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="1">
+        <v>0.23102749988902299</v>
+      </c>
+      <c r="C24" s="1">
+        <v>8.4280001465231104E-4</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2318702999036753</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -821,16 +825,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>2.9711085998424074</v>
+        <v>3.2021360997314305</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>2.2450419000378989</v>
+        <v>2.2458847000525513</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>5.2161504998803068</v>
+        <v>5.4480207997839818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 22 Solution (and 21 revised)
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -385,7 +385,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -756,15 +758,15 @@
         <v>21</v>
       </c>
       <c r="B25" s="1">
-        <v>7.9096517000580198</v>
+        <v>7.78277159994468</v>
       </c>
       <c r="C25" s="1">
-        <v>5.4889998864382505E-4</v>
+        <v>6.3530006445944298E-4</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>7.9102006000466636</v>
+        <v>7.7834069000091395</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -772,12 +774,16 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="1">
+        <v>27.250088499975298</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.0418000165373E-3</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27.251130299991836</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -827,16 +833,16 @@
     <row r="31" spans="1:5">
       <c r="B31" s="1">
         <f>SUM(B5:B29)</f>
-        <v>11.11178779978945</v>
+        <v>38.234996199651405</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C5:C29)</f>
-        <v>2.2464336000411951</v>
+        <v>2.247561800133548</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1">
         <f>SUM(E5:E29)</f>
-        <v>13.358221399830645</v>
+        <v>40.482557999784959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>